<commit_message>
Criando estrutura do histórico
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
@@ -774,106 +774,6 @@
       </spPr>
     </pic>
     <clientData fLocksWithSheet="0"/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>17</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>19</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>21</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>3</col>
-      <colOff>0</colOff>
-      <row>11</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="952500" cy="476250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
   </oneCellAnchor>
 </wsDr>
 </file>
@@ -1375,213 +1275,79 @@
       <c r="K17" s="88" t="n"/>
     </row>
     <row r="18" ht="57.75" customHeight="1" s="6">
-      <c r="A18" s="17" t="inlineStr">
-        <is>
-          <t>01/01/2025</t>
-        </is>
-      </c>
-      <c r="B18" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
+      <c r="A18" s="17" t="n"/>
+      <c r="B18" s="17" t="n"/>
       <c r="C18" s="85" t="n"/>
       <c r="D18" s="86" t="n"/>
-      <c r="E18" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-001</t>
-        </is>
-      </c>
+      <c r="E18" s="17" t="n"/>
       <c r="F18" s="86" t="n"/>
-      <c r="G18" s="18" t="inlineStr">
-        <is>
-          <t>0 - 600</t>
-        </is>
-      </c>
-      <c r="H18" s="61" t="inlineStr">
-        <is>
-          <t>Entrega</t>
-        </is>
-      </c>
+      <c r="G18" s="18" t="n"/>
+      <c r="H18" s="61" t="n"/>
       <c r="I18" s="17" t="n"/>
       <c r="J18" s="17" t="n"/>
       <c r="K18" s="86" t="n"/>
     </row>
-    <row r="19" ht="57.75" customHeight="1" s="6">
-      <c r="A19" s="17" t="inlineStr">
-        <is>
-          <t>06/01/2025</t>
-        </is>
-      </c>
-      <c r="B19" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C19" s="85" t="n"/>
-      <c r="D19" s="86" t="n"/>
-      <c r="E19" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-001</t>
-        </is>
-      </c>
-      <c r="F19" s="86" t="n"/>
-      <c r="G19" s="18" t="inlineStr">
-        <is>
-          <t>0 - 600</t>
-        </is>
-      </c>
-      <c r="H19" s="61" t="inlineStr">
-        <is>
-          <t>substituição</t>
-        </is>
-      </c>
-      <c r="I19" s="17" t="inlineStr">
-        <is>
-          <t>06/01/2025</t>
-        </is>
-      </c>
-      <c r="J19" s="17" t="n"/>
-      <c r="K19" s="86" t="n"/>
-    </row>
-    <row r="20" ht="57.75" customHeight="1" s="6">
-      <c r="A20" s="17" t="inlineStr">
-        <is>
-          <t>06/01/2025</t>
-        </is>
-      </c>
-      <c r="B20" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C20" s="85" t="n"/>
-      <c r="D20" s="86" t="n"/>
-      <c r="E20" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-002</t>
-        </is>
-      </c>
-      <c r="F20" s="86" t="n"/>
-      <c r="G20" s="18" t="inlineStr">
-        <is>
-          <t>0 - 120</t>
-        </is>
-      </c>
-      <c r="H20" s="61" t="inlineStr">
-        <is>
-          <t>Entrega - Temporária</t>
-        </is>
-      </c>
-      <c r="I20" s="17" t="n"/>
-      <c r="J20" s="17" t="n"/>
-      <c r="K20" s="86" t="n"/>
-    </row>
-    <row r="21" ht="57.75" customHeight="1" s="6">
-      <c r="A21" s="17" t="inlineStr">
-        <is>
-          <t>10/01/2025</t>
-        </is>
-      </c>
-      <c r="B21" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C21" s="85" t="n"/>
-      <c r="D21" s="86" t="n"/>
-      <c r="E21" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-002</t>
-        </is>
-      </c>
-      <c r="F21" s="86" t="n"/>
-      <c r="G21" s="18" t="inlineStr">
-        <is>
-          <t>0 - 120</t>
-        </is>
-      </c>
-      <c r="H21" s="61" t="inlineStr">
-        <is>
-          <t>devolução</t>
-        </is>
-      </c>
-      <c r="I21" s="17" t="inlineStr">
-        <is>
-          <t>10/01/2025</t>
-        </is>
-      </c>
-      <c r="J21" s="17" t="n"/>
-      <c r="K21" s="86" t="n"/>
-    </row>
-    <row r="22" ht="57.75" customHeight="1" s="6">
-      <c r="A22" s="17" t="inlineStr">
-        <is>
-          <t>16/01/2025</t>
-        </is>
-      </c>
-      <c r="B22" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C22" s="85" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-001</t>
-        </is>
-      </c>
-      <c r="F22" s="86" t="n"/>
-      <c r="G22" s="18" t="inlineStr">
-        <is>
-          <t>0 - 600</t>
-        </is>
-      </c>
-      <c r="H22" s="61" t="inlineStr">
-        <is>
-          <t>Entrega</t>
-        </is>
-      </c>
-      <c r="I22" s="17" t="n"/>
-      <c r="J22" s="17" t="n"/>
-      <c r="K22" s="86" t="n"/>
-    </row>
+    <row r="19" ht="12.75" customHeight="1" s="6">
+      <c r="A19" s="7" t="n"/>
+      <c r="B19" s="7" t="n"/>
+      <c r="C19" s="7" t="n"/>
+      <c r="E19" s="7" t="n"/>
+      <c r="F19" s="7" t="n"/>
+      <c r="G19" s="7" t="n"/>
+      <c r="H19" s="7" t="n"/>
+      <c r="I19" s="7" t="n"/>
+      <c r="J19" s="7" t="n"/>
+      <c r="K19" s="7" t="n"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="7" t="n"/>
+      <c r="C20" s="7" t="n"/>
+      <c r="E20" s="7" t="n"/>
+      <c r="F20" s="7" t="n"/>
+      <c r="G20" s="7" t="n"/>
+      <c r="H20" s="7" t="n"/>
+      <c r="I20" s="7" t="n"/>
+      <c r="J20" s="7" t="n"/>
+      <c r="K20" s="7" t="n"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="6">
+      <c r="A21" s="7" t="n"/>
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+      <c r="D21" s="7" t="n"/>
+      <c r="E21" s="7" t="n"/>
+      <c r="F21" s="7" t="n"/>
+      <c r="G21" s="7" t="n"/>
+      <c r="H21" s="7" t="n"/>
+      <c r="I21" s="7" t="n"/>
+      <c r="J21" s="7" t="n"/>
+      <c r="K21" s="7" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="6"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="24">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J19:K19"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A8:K10"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="J17:K17"/>

</xml_diff>

<commit_message>
Criando campo de histórico e finalizando designacao de mais de um instrumento
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
@@ -774,6 +774,106 @@
       </spPr>
     </pic>
     <clientData fLocksWithSheet="0"/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>18</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="952500" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
   </oneCellAnchor>
 </wsDr>
 </file>
@@ -1275,79 +1375,213 @@
       <c r="K17" s="88" t="n"/>
     </row>
     <row r="18" ht="57.75" customHeight="1" s="6">
-      <c r="A18" s="17" t="n"/>
-      <c r="B18" s="17" t="n"/>
+      <c r="A18" s="17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="B18" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
       <c r="C18" s="85" t="n"/>
       <c r="D18" s="86" t="n"/>
-      <c r="E18" s="17" t="n"/>
+      <c r="E18" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-001</t>
+        </is>
+      </c>
       <c r="F18" s="86" t="n"/>
-      <c r="G18" s="18" t="n"/>
-      <c r="H18" s="61" t="n"/>
-      <c r="I18" s="17" t="n"/>
+      <c r="G18" s="18" t="inlineStr">
+        <is>
+          <t>0 - 600</t>
+        </is>
+      </c>
+      <c r="H18" s="61" t="inlineStr">
+        <is>
+          <t>devolução</t>
+        </is>
+      </c>
+      <c r="I18" s="17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
       <c r="J18" s="17" t="n"/>
       <c r="K18" s="86" t="n"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1" s="6">
-      <c r="A19" s="7" t="n"/>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1" s="6">
-      <c r="A20" s="7" t="n"/>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1" s="6">
-      <c r="A21" s="7" t="n"/>
-      <c r="B21" s="7" t="n"/>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="n"/>
-      <c r="I21" s="7" t="n"/>
-      <c r="J21" s="7" t="n"/>
-      <c r="K21" s="7" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="6"/>
+    <row r="19" ht="57.75" customHeight="1" s="6">
+      <c r="A19" s="17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="B19" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C19" s="85" t="n"/>
+      <c r="D19" s="86" t="n"/>
+      <c r="E19" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-001</t>
+        </is>
+      </c>
+      <c r="F19" s="86" t="n"/>
+      <c r="G19" s="18" t="inlineStr">
+        <is>
+          <t>0 - 600</t>
+        </is>
+      </c>
+      <c r="H19" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I19" s="17" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="86" t="n"/>
+    </row>
+    <row r="20" ht="57.75" customHeight="1" s="6">
+      <c r="A20" s="17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="B20" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C20" s="85" t="n"/>
+      <c r="D20" s="86" t="n"/>
+      <c r="E20" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-004</t>
+        </is>
+      </c>
+      <c r="F20" s="86" t="n"/>
+      <c r="G20" s="18" t="inlineStr">
+        <is>
+          <t>0 - 750</t>
+        </is>
+      </c>
+      <c r="H20" s="61" t="inlineStr">
+        <is>
+          <t>entrega</t>
+        </is>
+      </c>
+      <c r="I20" s="17" t="n"/>
+      <c r="J20" s="17" t="n"/>
+      <c r="K20" s="86" t="n"/>
+    </row>
+    <row r="21" ht="57.75" customHeight="1" s="6">
+      <c r="A21" s="17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="B21" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C21" s="85" t="n"/>
+      <c r="D21" s="86" t="n"/>
+      <c r="E21" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-003</t>
+        </is>
+      </c>
+      <c r="F21" s="86" t="n"/>
+      <c r="G21" s="18" t="inlineStr">
+        <is>
+          <t>0 - 700, 0 - 750</t>
+        </is>
+      </c>
+      <c r="H21" s="61" t="inlineStr">
+        <is>
+          <t>entrega</t>
+        </is>
+      </c>
+      <c r="I21" s="17" t="n"/>
+      <c r="J21" s="17" t="n"/>
+      <c r="K21" s="86" t="n"/>
+    </row>
+    <row r="22" ht="57.75" customHeight="1" s="6">
+      <c r="A22" s="17" t="inlineStr">
+        <is>
+          <t>04/02/2025</t>
+        </is>
+      </c>
+      <c r="B22" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C22" s="85" t="n"/>
+      <c r="D22" s="86" t="n"/>
+      <c r="E22" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-004</t>
+        </is>
+      </c>
+      <c r="F22" s="86" t="n"/>
+      <c r="G22" s="18" t="inlineStr">
+        <is>
+          <t>0 - 750</t>
+        </is>
+      </c>
+      <c r="H22" s="61" t="inlineStr">
+        <is>
+          <t>devolução</t>
+        </is>
+      </c>
+      <c r="I22" s="17" t="inlineStr">
+        <is>
+          <t>04/02/2025</t>
+        </is>
+      </c>
+      <c r="J22" s="17" t="n"/>
+      <c r="K22" s="86" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="36">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="J19:K19"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A8:K10"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="J17:K17"/>

</xml_diff>

<commit_message>
Add histórico e crud
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
@@ -774,106 +774,6 @@
       </spPr>
     </pic>
     <clientData fLocksWithSheet="0"/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>18</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>19</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>20</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>3</col>
-      <colOff>0</colOff>
-      <row>11</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="952500" cy="476250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
   </oneCellAnchor>
 </wsDr>
 </file>
@@ -1375,213 +1275,79 @@
       <c r="K17" s="88" t="n"/>
     </row>
     <row r="18" ht="57.75" customHeight="1" s="6">
-      <c r="A18" s="17" t="inlineStr">
-        <is>
-          <t>03/02/2025</t>
-        </is>
-      </c>
-      <c r="B18" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
+      <c r="A18" s="17" t="n"/>
+      <c r="B18" s="17" t="n"/>
       <c r="C18" s="85" t="n"/>
       <c r="D18" s="86" t="n"/>
-      <c r="E18" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-001</t>
-        </is>
-      </c>
+      <c r="E18" s="17" t="n"/>
       <c r="F18" s="86" t="n"/>
-      <c r="G18" s="18" t="inlineStr">
-        <is>
-          <t>0 - 600</t>
-        </is>
-      </c>
-      <c r="H18" s="61" t="inlineStr">
-        <is>
-          <t>devolução</t>
-        </is>
-      </c>
-      <c r="I18" s="17" t="inlineStr">
-        <is>
-          <t>03/02/2025</t>
-        </is>
-      </c>
+      <c r="G18" s="18" t="n"/>
+      <c r="H18" s="61" t="n"/>
+      <c r="I18" s="17" t="n"/>
       <c r="J18" s="17" t="n"/>
       <c r="K18" s="86" t="n"/>
     </row>
-    <row r="19" ht="57.75" customHeight="1" s="6">
-      <c r="A19" s="17" t="inlineStr">
-        <is>
-          <t>03/02/2025</t>
-        </is>
-      </c>
-      <c r="B19" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C19" s="85" t="n"/>
-      <c r="D19" s="86" t="n"/>
-      <c r="E19" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-001</t>
-        </is>
-      </c>
-      <c r="F19" s="86" t="n"/>
-      <c r="G19" s="18" t="inlineStr">
-        <is>
-          <t>0 - 600</t>
-        </is>
-      </c>
-      <c r="H19" s="61" t="inlineStr">
-        <is>
-          <t>Entrega</t>
-        </is>
-      </c>
-      <c r="I19" s="17" t="n"/>
-      <c r="J19" s="17" t="n"/>
-      <c r="K19" s="86" t="n"/>
-    </row>
-    <row r="20" ht="57.75" customHeight="1" s="6">
-      <c r="A20" s="17" t="inlineStr">
-        <is>
-          <t>03/02/2025</t>
-        </is>
-      </c>
-      <c r="B20" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C20" s="85" t="n"/>
-      <c r="D20" s="86" t="n"/>
-      <c r="E20" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-004</t>
-        </is>
-      </c>
-      <c r="F20" s="86" t="n"/>
-      <c r="G20" s="18" t="inlineStr">
-        <is>
-          <t>0 - 750</t>
-        </is>
-      </c>
-      <c r="H20" s="61" t="inlineStr">
-        <is>
-          <t>entrega</t>
-        </is>
-      </c>
-      <c r="I20" s="17" t="n"/>
-      <c r="J20" s="17" t="n"/>
-      <c r="K20" s="86" t="n"/>
-    </row>
-    <row r="21" ht="57.75" customHeight="1" s="6">
-      <c r="A21" s="17" t="inlineStr">
-        <is>
-          <t>03/02/2025</t>
-        </is>
-      </c>
-      <c r="B21" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C21" s="85" t="n"/>
-      <c r="D21" s="86" t="n"/>
-      <c r="E21" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-003</t>
-        </is>
-      </c>
-      <c r="F21" s="86" t="n"/>
-      <c r="G21" s="18" t="inlineStr">
-        <is>
-          <t>0 - 700, 0 - 750</t>
-        </is>
-      </c>
-      <c r="H21" s="61" t="inlineStr">
-        <is>
-          <t>entrega</t>
-        </is>
-      </c>
-      <c r="I21" s="17" t="n"/>
-      <c r="J21" s="17" t="n"/>
-      <c r="K21" s="86" t="n"/>
-    </row>
-    <row r="22" ht="57.75" customHeight="1" s="6">
-      <c r="A22" s="17" t="inlineStr">
-        <is>
-          <t>04/02/2025</t>
-        </is>
-      </c>
-      <c r="B22" s="17" t="inlineStr">
-        <is>
-          <t>Paquímetro analógico</t>
-        </is>
-      </c>
-      <c r="C22" s="85" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="17" t="inlineStr">
-        <is>
-          <t>PAQ-004</t>
-        </is>
-      </c>
-      <c r="F22" s="86" t="n"/>
-      <c r="G22" s="18" t="inlineStr">
-        <is>
-          <t>0 - 750</t>
-        </is>
-      </c>
-      <c r="H22" s="61" t="inlineStr">
-        <is>
-          <t>devolução</t>
-        </is>
-      </c>
-      <c r="I22" s="17" t="inlineStr">
-        <is>
-          <t>04/02/2025</t>
-        </is>
-      </c>
-      <c r="J22" s="17" t="n"/>
-      <c r="K22" s="86" t="n"/>
-    </row>
+    <row r="19" ht="12.75" customHeight="1" s="6">
+      <c r="A19" s="7" t="n"/>
+      <c r="B19" s="7" t="n"/>
+      <c r="C19" s="7" t="n"/>
+      <c r="E19" s="7" t="n"/>
+      <c r="F19" s="7" t="n"/>
+      <c r="G19" s="7" t="n"/>
+      <c r="H19" s="7" t="n"/>
+      <c r="I19" s="7" t="n"/>
+      <c r="J19" s="7" t="n"/>
+      <c r="K19" s="7" t="n"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="7" t="n"/>
+      <c r="C20" s="7" t="n"/>
+      <c r="E20" s="7" t="n"/>
+      <c r="F20" s="7" t="n"/>
+      <c r="G20" s="7" t="n"/>
+      <c r="H20" s="7" t="n"/>
+      <c r="I20" s="7" t="n"/>
+      <c r="J20" s="7" t="n"/>
+      <c r="K20" s="7" t="n"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="6">
+      <c r="A21" s="7" t="n"/>
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+      <c r="D21" s="7" t="n"/>
+      <c r="E21" s="7" t="n"/>
+      <c r="F21" s="7" t="n"/>
+      <c r="G21" s="7" t="n"/>
+      <c r="H21" s="7" t="n"/>
+      <c r="I21" s="7" t="n"/>
+      <c r="J21" s="7" t="n"/>
+      <c r="K21" s="7" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="6"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="24">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J19:K19"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A8:K10"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="J17:K17"/>

</xml_diff>

<commit_message>
Sunbindo BD prod e ajustando desempenho do sistema
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
@@ -774,6 +774,156 @@
       </spPr>
     </pic>
     <clientData fLocksWithSheet="0"/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="952500" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
   </oneCellAnchor>
 </wsDr>
 </file>
@@ -980,7 +1130,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -1275,80 +1425,286 @@
       <c r="K17" s="88" t="n"/>
     </row>
     <row r="18" ht="57.75" customHeight="1" s="6">
-      <c r="A18" s="17" t="n"/>
-      <c r="B18" s="17" t="n"/>
+      <c r="A18" s="17" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="B18" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
       <c r="C18" s="85" t="n"/>
       <c r="D18" s="86" t="n"/>
-      <c r="E18" s="17" t="n"/>
+      <c r="E18" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-004</t>
+        </is>
+      </c>
       <c r="F18" s="86" t="n"/>
-      <c r="G18" s="18" t="n"/>
-      <c r="H18" s="61" t="n"/>
+      <c r="G18" s="18" t="inlineStr">
+        <is>
+          <t>0 - 750</t>
+        </is>
+      </c>
+      <c r="H18" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
       <c r="I18" s="17" t="n"/>
       <c r="J18" s="17" t="n"/>
       <c r="K18" s="86" t="n"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1" s="6">
-      <c r="A19" s="7" t="n"/>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1" s="6">
-      <c r="A20" s="7" t="n"/>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1" s="6">
-      <c r="A21" s="7" t="n"/>
-      <c r="B21" s="7" t="n"/>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="n"/>
-      <c r="I21" s="7" t="n"/>
-      <c r="J21" s="7" t="n"/>
-      <c r="K21" s="7" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="6"/>
+    <row r="19" ht="57.75" customHeight="1" s="6">
+      <c r="A19" s="17" t="inlineStr">
+        <is>
+          <t>10/02/2025</t>
+        </is>
+      </c>
+      <c r="B19" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C19" s="85" t="n"/>
+      <c r="D19" s="86" t="n"/>
+      <c r="E19" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-004</t>
+        </is>
+      </c>
+      <c r="F19" s="86" t="n"/>
+      <c r="G19" s="18" t="inlineStr">
+        <is>
+          <t>0 - 750</t>
+        </is>
+      </c>
+      <c r="H19" s="61" t="inlineStr">
+        <is>
+          <t>devolução - None</t>
+        </is>
+      </c>
+      <c r="I19" s="17" t="inlineStr">
+        <is>
+          <t>10/02/2025</t>
+        </is>
+      </c>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="86" t="n"/>
+    </row>
+    <row r="20" ht="57.75" customHeight="1" s="6">
+      <c r="A20" s="17" t="inlineStr">
+        <is>
+          <t>19/02/2025</t>
+        </is>
+      </c>
+      <c r="B20" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C20" s="85" t="n"/>
+      <c r="D20" s="86" t="n"/>
+      <c r="E20" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-001</t>
+        </is>
+      </c>
+      <c r="F20" s="86" t="n"/>
+      <c r="G20" s="18" t="inlineStr">
+        <is>
+          <t>0 - 600</t>
+        </is>
+      </c>
+      <c r="H20" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I20" s="17" t="n"/>
+      <c r="J20" s="17" t="n"/>
+      <c r="K20" s="86" t="n"/>
+    </row>
+    <row r="21" ht="57.75" customHeight="1" s="6">
+      <c r="A21" s="17" t="inlineStr">
+        <is>
+          <t>19/02/2025</t>
+        </is>
+      </c>
+      <c r="B21" s="17" t="inlineStr">
+        <is>
+          <t>Manômetro</t>
+        </is>
+      </c>
+      <c r="C21" s="85" t="n"/>
+      <c r="D21" s="86" t="n"/>
+      <c r="E21" s="17" t="inlineStr">
+        <is>
+          <t>MAN-CQ-001</t>
+        </is>
+      </c>
+      <c r="F21" s="86" t="n"/>
+      <c r="G21" s="18" t="inlineStr">
+        <is>
+          <t>0 - 700</t>
+        </is>
+      </c>
+      <c r="H21" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I21" s="17" t="n"/>
+      <c r="J21" s="17" t="n"/>
+      <c r="K21" s="86" t="n"/>
+    </row>
+    <row r="22" ht="57.75" customHeight="1" s="6">
+      <c r="A22" s="17" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B22" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C22" s="85" t="n"/>
+      <c r="D22" s="86" t="n"/>
+      <c r="E22" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-001</t>
+        </is>
+      </c>
+      <c r="F22" s="86" t="n"/>
+      <c r="G22" s="18" t="inlineStr">
+        <is>
+          <t>0 - 600</t>
+        </is>
+      </c>
+      <c r="H22" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I22" s="17" t="n"/>
+      <c r="J22" s="17" t="n"/>
+      <c r="K22" s="86" t="n"/>
+    </row>
+    <row r="23" ht="57.75" customHeight="1" s="6">
+      <c r="A23" s="17" t="inlineStr">
+        <is>
+          <t>03/03/2025</t>
+        </is>
+      </c>
+      <c r="B23" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C23" s="85" t="n"/>
+      <c r="D23" s="86" t="n"/>
+      <c r="E23" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-001</t>
+        </is>
+      </c>
+      <c r="F23" s="86" t="n"/>
+      <c r="G23" s="18" t="inlineStr">
+        <is>
+          <t>0 - 600</t>
+        </is>
+      </c>
+      <c r="H23" s="61" t="inlineStr">
+        <is>
+          <t>substituição - calibração</t>
+        </is>
+      </c>
+      <c r="I23" s="17" t="inlineStr">
+        <is>
+          <t>03/03/2025</t>
+        </is>
+      </c>
+      <c r="J23" s="17" t="n"/>
+      <c r="K23" s="86" t="n"/>
+    </row>
+    <row r="24" ht="57.75" customHeight="1" s="6">
+      <c r="A24" s="17" t="inlineStr">
+        <is>
+          <t>03/03/2025</t>
+        </is>
+      </c>
+      <c r="B24" s="17" t="inlineStr">
+        <is>
+          <t>Paquímetro analógico</t>
+        </is>
+      </c>
+      <c r="C24" s="85" t="n"/>
+      <c r="D24" s="86" t="n"/>
+      <c r="E24" s="17" t="inlineStr">
+        <is>
+          <t>PAQ-002</t>
+        </is>
+      </c>
+      <c r="F24" s="86" t="n"/>
+      <c r="G24" s="18" t="inlineStr">
+        <is>
+          <t>0 - 120</t>
+        </is>
+      </c>
+      <c r="H24" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I24" s="17" t="n"/>
+      <c r="J24" s="17" t="n"/>
+      <c r="K24" s="86" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="42">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A8:K10"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="H7:K7"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="J17:K17"/>
   </mergeCells>

</xml_diff>

<commit_message>
:sparkles: feat: Editar certificado
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-Luan Araújo.xlsx
@@ -802,56 +802,6 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>19</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>21</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1619250" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
       <col>3</col>
       <colOff>0</colOff>
       <row>11</row>
@@ -860,11 +810,11 @@
     <ext cx="952500" cy="476250"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1247,7 +1197,7 @@
       </c>
       <c r="H7" s="52" t="inlineStr">
         <is>
-          <t>Corte e estamparia</t>
+          <t>Corte e Estamparia</t>
         </is>
       </c>
       <c r="I7" s="81" t="n"/>
@@ -1377,7 +1327,7 @@
     <row r="18" ht="57.75" customHeight="1" s="6">
       <c r="A18" s="17" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B18" s="17" t="inlineStr">
@@ -1410,7 +1360,7 @@
     <row r="19" ht="57.75" customHeight="1" s="6">
       <c r="A19" s="17" t="inlineStr">
         <is>
-          <t>17/02/2025</t>
+          <t>23/06/2025</t>
         </is>
       </c>
       <c r="B19" s="17" t="inlineStr">
@@ -1438,117 +1388,40 @@
       </c>
       <c r="I19" s="17" t="inlineStr">
         <is>
-          <t>17/02/2025</t>
+          <t>23/06/2025</t>
         </is>
       </c>
       <c r="J19" s="17" t="n"/>
       <c r="K19" s="86" t="n"/>
     </row>
-    <row r="20" ht="57.75" customHeight="1" s="6">
-      <c r="A20" s="17" t="inlineStr">
-        <is>
-          <t>24/02/2025</t>
-        </is>
-      </c>
-      <c r="B20" s="17" t="inlineStr">
-        <is>
-          <t>Trena</t>
-        </is>
-      </c>
-      <c r="C20" s="85" t="n"/>
-      <c r="D20" s="86" t="n"/>
-      <c r="E20" s="17" t="inlineStr">
-        <is>
-          <t>TRE-CQ-048</t>
-        </is>
-      </c>
-      <c r="F20" s="86" t="n"/>
-      <c r="G20" s="18" t="inlineStr">
-        <is>
-          <t>0 - 400, 0 - 380</t>
-        </is>
-      </c>
-      <c r="H20" s="61" t="inlineStr">
-        <is>
-          <t>Entrega</t>
-        </is>
-      </c>
-      <c r="I20" s="17" t="n"/>
-      <c r="J20" s="17" t="n"/>
-      <c r="K20" s="86" t="n"/>
-    </row>
-    <row r="21" ht="57.75" customHeight="1" s="6">
-      <c r="A21" s="17" t="inlineStr">
-        <is>
-          <t>25/02/2025</t>
-        </is>
-      </c>
-      <c r="B21" s="17" t="inlineStr">
-        <is>
-          <t>Trena</t>
-        </is>
-      </c>
-      <c r="C21" s="85" t="n"/>
-      <c r="D21" s="86" t="n"/>
-      <c r="E21" s="17" t="inlineStr">
-        <is>
-          <t>TRE-CQ-048</t>
-        </is>
-      </c>
-      <c r="F21" s="86" t="n"/>
-      <c r="G21" s="18" t="inlineStr">
-        <is>
-          <t>0 - 400, 0 - 380</t>
-        </is>
-      </c>
-      <c r="H21" s="61" t="inlineStr">
-        <is>
-          <t>substituição - calibração</t>
-        </is>
-      </c>
-      <c r="I21" s="17" t="inlineStr">
-        <is>
-          <t>25/02/2025</t>
-        </is>
-      </c>
-      <c r="J21" s="17" t="n"/>
-      <c r="K21" s="86" t="n"/>
-    </row>
-    <row r="22" ht="57.75" customHeight="1" s="6">
-      <c r="A22" s="17" t="inlineStr">
-        <is>
-          <t>25/02/2025</t>
-        </is>
-      </c>
-      <c r="B22" s="17" t="inlineStr">
-        <is>
-          <t>Trena</t>
-        </is>
-      </c>
-      <c r="C22" s="85" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="17" t="inlineStr">
-        <is>
-          <t>TRE-CQ-056</t>
-        </is>
-      </c>
-      <c r="F22" s="86" t="n"/>
-      <c r="G22" s="18" t="inlineStr">
-        <is>
-          <t>0 - 400</t>
-        </is>
-      </c>
-      <c r="H22" s="61" t="inlineStr">
-        <is>
-          <t>Entrega</t>
-        </is>
-      </c>
-      <c r="I22" s="17" t="n"/>
-      <c r="J22" s="17" t="n"/>
-      <c r="K22" s="86" t="n"/>
-    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="7" t="n"/>
+      <c r="C20" s="7" t="n"/>
+      <c r="E20" s="7" t="n"/>
+      <c r="F20" s="7" t="n"/>
+      <c r="G20" s="7" t="n"/>
+      <c r="H20" s="7" t="n"/>
+      <c r="I20" s="7" t="n"/>
+      <c r="J20" s="7" t="n"/>
+      <c r="K20" s="7" t="n"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="6">
+      <c r="A21" s="7" t="n"/>
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+      <c r="D21" s="7" t="n"/>
+      <c r="E21" s="7" t="n"/>
+      <c r="F21" s="7" t="n"/>
+      <c r="G21" s="7" t="n"/>
+      <c r="H21" s="7" t="n"/>
+      <c r="I21" s="7" t="n"/>
+      <c r="J21" s="7" t="n"/>
+      <c r="K21" s="7" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="6"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="27">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="H1:I1"/>
@@ -1559,29 +1432,20 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A8:K10"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="J17:K17"/>

</xml_diff>